<commit_message>
change dcl case as the db column name changed by developer
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
@@ -205,23 +205,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select host,`user`,AUTHENTICATION_STRING from mysql.user where `user`='dcltest1'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select host,`user`,AUTHENTICATION_STRING from mysql.user where `user`='dcltest2'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select host,`user`,AUTHENTICATION_STRING from mysql.user where `user`='dcltest3'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select `user`,AUTHENTICATION_STRING from mysql.user where `user`='dcltest4'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>create user 'dcltest4'@'localhost' identified by 'abc123'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,name,AUTHENTICATION_STRING from mysql.user where name='dcltest1'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,name,AUTHENTICATION_STRING from mysql.user where name='dcltest2'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,name,AUTHENTICATION_STRING from mysql.user where name='dcltest3'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select name,AUTHENTICATION_STRING from mysql.user where name='dcltest4'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -595,7 +595,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -714,7 +714,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>25</v>
@@ -752,7 +752,7 @@
         <v>39</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>33</v>
@@ -790,7 +790,7 @@
         <v>40</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>41</v>
@@ -825,10 +825,10 @@
         <v>48</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
add dcl revoke and reset password case
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="149">
   <si>
     <t>TestID</t>
   </si>
@@ -51,23 +51,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Query_user</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Expected_user</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Query_db</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Expected_db</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_tablesPriv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -475,6 +463,110 @@
   </si>
   <si>
     <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where name='dcltest7' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcl_008</t>
+  </si>
+  <si>
+    <t>修改用户密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcltest8</t>
+  </si>
+  <si>
+    <t>create user 'dcltest8' identified by 'abc123'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_tablesPriv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reset_pass_str</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>def456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcl_009</t>
+  </si>
+  <si>
+    <t>给用户赋单一权限select后，收回权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dcltest9</t>
+  </si>
+  <si>
+    <t>abc123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Revoke_state</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,name from mysql.user where name='dcltest9'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dcl/expectedresult/user/dcl_009.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dcl/expectedresult/db/dcl_009.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest9' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grant select on dingo.studentdc to 'dcltest9'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dcl/expectedresult/tables_priv/dcl_009.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show grants for 'dcltest9'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dcl/expectedresult/grants/dcl_009.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create user 'dcltest9' identified by 'abc123'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where name='dcltest9' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>revoke select on dingo.studentdc from 'dcltest9'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dcl/expectedresult/revokegrants/dcl_009.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected_grants_after_revoke</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -846,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -860,25 +952,26 @@
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5" style="4" customWidth="1"/>
-    <col min="12" max="12" width="19.5" style="5" customWidth="1"/>
-    <col min="13" max="13" width="21.75" style="4" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="5" customWidth="1"/>
-    <col min="15" max="15" width="42.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5" style="4" customWidth="1"/>
-    <col min="18" max="18" width="21.75" style="4" customWidth="1"/>
-    <col min="19" max="19" width="28" style="4" customWidth="1"/>
-    <col min="20" max="20" width="19.5" style="4" customWidth="1"/>
-    <col min="21" max="21" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="18.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.75" style="1" customWidth="1"/>
+    <col min="10" max="10" width="25" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" style="4" customWidth="1"/>
+    <col min="13" max="13" width="19.5" style="5" customWidth="1"/>
+    <col min="14" max="14" width="21.75" style="4" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="5" customWidth="1"/>
+    <col min="16" max="16" width="42.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="19.5" style="4" customWidth="1"/>
+    <col min="21" max="21" width="21.75" style="4" customWidth="1"/>
+    <col min="22" max="22" width="28" style="4" customWidth="1"/>
+    <col min="23" max="23" width="19.5" style="4" customWidth="1"/>
+    <col min="24" max="24" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -892,58 +985,67 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="N1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="U1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -957,396 +1059,494 @@
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>89</v>
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>75</v>
+        <v>26</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>72</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>59</v>
+        <v>17</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>76</v>
+        <v>56</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>73</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>61</v>
+        <v>17</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>77</v>
+        <v>58</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="S6" s="4" t="s">
+      <c r="R6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="L7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="M7" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="N7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="N7" s="5" t="s">
+      <c r="R7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="P7" s="4" t="s">
+      <c r="U7" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="V7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="R7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U7" s="1" t="s">
+      <c r="W7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="L8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="N8" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="R8" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="K8" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="R8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="U8" s="1" t="s">
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="W9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1356,10 +1556,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"y,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X1048576">
       <formula1>"effected_rows_assert,csv_equals,csv_containsAll,string_equals,SQLException,assertNull"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update mysql protocol test case result and change user column name
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
@@ -477,76 +477,94 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select host,name,AUTHENTICATION_STRING from mysql.user where name='dcltest1'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where name='dcltest1' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest1' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,AUTHENTICATION_STRING from mysql.user where name='dcltest2'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where name='dcltest2' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest2' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,AUTHENTICATION_STRING from mysql.user where name='dcltest3'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where name='dcltest3' and host='172.20.3.27'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest3' and host='172.20.3.27'</t>
-  </si>
-  <si>
-    <t>select name,AUTHENTICATION_STRING from mysql.user where name='dcltest4'</t>
-  </si>
-  <si>
-    <t>select name,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where name='dcltest4'</t>
-  </si>
-  <si>
-    <t>select name,db,table_name,table_priv from mysql.tables_priv where name='dcltest4'</t>
-  </si>
-  <si>
-    <t>select host,name from mysql.user where name='dcltest5'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where name='dcltest5' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest5' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.user where name='dcltest6' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where name='dcltest6' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest6' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv,reload_priv,shutdown_priv,PROCESS_PRIV,FILE_PRIV,GRANT_PRIV,REFERENCES_PRIV,INDEX_PRIV,SHOW_DB_PRIV,CREATE_USER_PRIV from mysql.user where name='dcltest7'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where name='dcltest7' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest7' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name from mysql.user where name='dcltest9'</t>
-  </si>
-  <si>
-    <t>select host,name,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where name='dcltest9' and host='%'</t>
-  </si>
-  <si>
-    <t>select host,name,db,table_name,table_priv from mysql.tables_priv where name='dcltest9' and host='%'</t>
+    <t>select host,user,AUTHENTICATION_STRING from mysql.user where user='dcltest1'</t>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where user='dcltest1' and host='%'</t>
+  </si>
+  <si>
+    <t>select host,user,AUTHENTICATION_STRING from mysql.user where user='dcltest2'</t>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where user='dcltest2' and host='%'</t>
+  </si>
+  <si>
+    <t>select host,user,AUTHENTICATION_STRING from mysql.user where user='dcltest3'</t>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where user='dcltest3' and host='172.20.3.27'</t>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest1' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest2' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest3' and host='172.20.3.27'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select user,db,table_name,table_priv from mysql.tables_priv where user='dcltest4'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest5' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest6' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest7' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,table_name,table_priv from mysql.tables_priv where user='dcltest9' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select user,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where user='dcltest4'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv from mysql.db where user='dcltest5' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where user='dcltest6' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where user='dcltest7' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,db,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.db where user='dcltest9' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select user,AUTHENTICATION_STRING from mysql.user where user='dcltest4'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user from mysql.user where user='dcltest5'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv from mysql.user where user='dcltest6' and host='%'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user,select_priv,insert_priv,update_priv,delete_priv,create_priv,drop_priv,reload_priv,shutdown_priv,PROCESS_PRIV,FILE_PRIV,GRANT_PRIV,REFERENCES_PRIV,INDEX_PRIV,SHOW_DB_PRIV,CREATE_USER_PRIV from mysql.user where user='dcltest7'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select host,user from mysql.user where user='dcltest9'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -920,7 +938,7 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1059,7 +1077,7 @@
         <v>71</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>67</v>
@@ -1103,19 +1121,19 @@
         <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>44</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>68</v>
@@ -1159,13 +1177,13 @@
         <v>51</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>45</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>64</v>
@@ -1215,19 +1233,19 @@
         <v>53</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>46</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>65</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>70</v>
@@ -1268,19 +1286,19 @@
         <v>41</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>62</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>66</v>
@@ -1330,7 +1348,7 @@
         <v>78</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>79</v>
@@ -1342,7 +1360,7 @@
         <v>80</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>81</v>
@@ -1392,19 +1410,19 @@
         <v>92</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>93</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>94</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>95</v>
@@ -1484,19 +1502,19 @@
         <v>121</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>115</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>116</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
change get tables size
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dcl/sql_dcl_cases.xlsx
@@ -381,10 +381,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>studentdc,classesdc,GLOBAL_VARIABLES,DB,TABLES_PRIV,USER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>dcl_008</t>
   </si>
   <si>
@@ -564,6 +560,10 @@
   </si>
   <si>
     <t>select host,user from mysql.user where user='dcltest9'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>studentdc,classesdc,GLOBAL_VARIABLES,DB,TABLES_PRIV,USER,COLUMNS,EVENTS,KEY_COLUMN_USAGE,PARTITIONS,ROUTINES,SCHEMATA,STATISTICS,TABLES,TRIGGERS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -988,7 +988,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>30</v>
@@ -997,19 +997,19 @@
         <v>14</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>12</v>
@@ -1024,10 +1024,10 @@
         <v>61</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>74</v>
@@ -1065,19 +1065,19 @@
         <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>71</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>67</v>
@@ -1121,19 +1121,19 @@
         <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>44</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>68</v>
@@ -1177,19 +1177,19 @@
         <v>51</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>45</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>64</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O4" s="5" t="s">
         <v>69</v>
@@ -1233,19 +1233,19 @@
         <v>53</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>46</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>65</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>70</v>
@@ -1286,19 +1286,19 @@
         <v>41</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>47</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>62</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O6" s="5" t="s">
         <v>66</v>
@@ -1348,19 +1348,19 @@
         <v>78</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>80</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>81</v>
@@ -1410,19 +1410,19 @@
         <v>92</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>93</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>94</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>95</v>
@@ -1437,7 +1437,7 @@
         <v>98</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="V8" s="2" t="s">
         <v>99</v>
@@ -1451,28 +1451,28 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J9" s="4"/>
       <c r="W9" s="4" t="s">
@@ -1481,58 +1481,58 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="I10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="S10" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>85</v>

</xml_diff>